<commit_message>
Added more products info
</commit_message>
<xml_diff>
--- a/graph_rolls.xlsx
+++ b/graph_rolls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d2f680566644eda/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{A34CB8AF-AA14-4F4F-A1E5-A14A4BFD8A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBC9E720-12D2-4B8A-9C9D-B7B98E4420F8}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{A34CB8AF-AA14-4F4F-A1E5-A14A4BFD8A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F314617-914D-403A-B6B9-AFE16FB92205}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3C6A63BF-2086-48D2-9BBD-07F76897DA4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C6A63BF-2086-48D2-9BBD-07F76897DA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="indefinite_chill" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,6 @@
     <sheet name="Adamite" sheetId="3" r:id="rId3"/>
     <sheet name="Forged" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">SG!$K$6:$K$25</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">SG!$L$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">SG!$L$6:$L$25</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">SG!$M$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">SG!$M$6:$M$25</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">SG!$N$5</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">SG!$N$6:$N$25</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">SG!$O$5</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">SG!$O$6:$O$25</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="121">
   <si>
     <t>Indefinite Chilled Cast Iron Rolls</t>
   </si>
@@ -263,18 +252,6 @@
     <t>depth</t>
   </si>
   <si>
-    <t>SGP1</t>
-  </si>
-  <si>
-    <t>SGP2</t>
-  </si>
-  <si>
-    <t>SGA1</t>
-  </si>
-  <si>
-    <t>SGA2</t>
-  </si>
-  <si>
     <t>Adamite Rolls</t>
   </si>
   <si>
@@ -330,15 +307,6 @@
   </si>
   <si>
     <t>AD2</t>
-  </si>
-  <si>
-    <t>ICC1</t>
-  </si>
-  <si>
-    <t>ICC2</t>
-  </si>
-  <si>
-    <t>ICC3</t>
   </si>
   <si>
     <t>Forged Rolls</t>
@@ -622,6 +590,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -661,9 +638,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -671,12 +645,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -816,13 +784,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -897,13 +865,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -978,13 +946,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1059,13 +1027,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1140,13 +1108,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1225,13 +1193,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1322,13 +1290,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>ICC1</c:v>
+                  <c:v>ICR1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ICC2</c:v>
+                  <c:v>ICR2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ICC3</c:v>
+                  <c:v>ICR3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1625,6 +1593,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="101702239"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3763,6 +3732,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1962638383"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5595,15 +5565,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>4760</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>309560</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6012,8 +5982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ED94A7-2BB9-4B78-8328-1FD1638AD682}">
   <dimension ref="A2:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6038,12 +6008,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
       <c r="I4" t="s">
         <v>33</v>
       </c>
@@ -6083,7 +6053,7 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="J5">
         <v>55</v>
@@ -6121,7 +6091,7 @@
         <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="J6">
         <v>60</v>
@@ -6159,7 +6129,7 @@
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="J7">
         <v>65</v>
@@ -6226,12 +6196,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -6251,11 +6221,11 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6273,8 +6243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860C5091-0069-44B5-B70F-8A9676751E4B}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6286,41 +6256,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="15"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="4" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -6359,16 +6329,16 @@
         <v>73</v>
       </c>
       <c r="L5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="M5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="N5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="O5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -6564,13 +6534,13 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="K12">
         <v>18</v>
       </c>
@@ -6842,23 +6812,23 @@
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="18"/>
+      <c r="D26" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -6997,13 +6967,13 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -7072,28 +7042,28 @@
   <sheetData>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>95</v>
+      <c r="A4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>79</v>
+      <c r="A5" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="I5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
         <v>26</v>
@@ -7122,16 +7092,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J6">
         <v>43</v>
@@ -7169,7 +7139,7 @@
         <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J7">
         <v>47</v>
@@ -7207,7 +7177,7 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J8">
         <v>52</v>
@@ -7236,13 +7206,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7253,10 +7223,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7270,29 +7240,29 @@
         <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7300,13 +7270,13 @@
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -7323,7 +7293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FF6F65-2C6B-489D-8D28-57D20E12F1EB}">
   <dimension ref="A3:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -7335,60 +7305,60 @@
   <sheetData>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>106</v>
+      <c r="A4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="A5" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7396,22 +7366,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7419,7 +7389,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -7428,18 +7398,18 @@
         <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B9" s="3">
         <v>0.05</v>
@@ -7488,22 +7458,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7511,22 +7481,22 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7534,22 +7504,22 @@
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>